<commit_message>
fix the two panels to be even & resizable
</commit_message>
<xml_diff>
--- a/testset/C2PA-JPT Testfiles.xlsx
+++ b/testset/C2PA-JPT Testfiles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/Development/c2pa-testfile-maker/testset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/Development/crTool/testset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38065CF4-47A6-C44A-A781-78AD2A5EA626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84693926-D4C3-B145-80C6-4E55ACEDBB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="71200" yWindow="8000" windowWidth="30080" windowHeight="25840" xr2:uid="{8EA77C23-A43E-9342-9FFB-5C3237DC0EFB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="68">
   <si>
     <t>Test Type</t>
   </si>
@@ -638,7 +638,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1281,6 +1281,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>

</xml_diff>